<commit_message>
Start to setup new DBC files
</commit_message>
<xml_diff>
--- a/matlab_code/F28379D/F28379D_benchTest/CANmailboxUsage.xlsx
+++ b/matlab_code/F28379D/F28379D_benchTest/CANmailboxUsage.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ETC-Development\matlab_code\etc_benchTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ETC-Development\matlab_code\F28379D\F28379D_benchTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991219C5-3A76-42CD-8393-936F6F66B624}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99784EA2-2331-47DB-9781-DFA291D4E138}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CAN IDs" sheetId="2" r:id="rId1"/>
+    <sheet name="Mailboxes" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Mailbox Number</t>
   </si>
@@ -39,39 +40,44 @@
     <t>CCP</t>
   </si>
   <si>
-    <t>Output</t>
+    <t>CPU</t>
   </si>
   <si>
-    <t>HI_VectorBox</t>
+    <t>CAN Message ID Reservations</t>
   </si>
   <si>
-    <t>Input</t>
+    <t>IDs</t>
   </si>
   <si>
-    <t>HO_CAN/Faults</t>
+    <t>Device</t>
   </si>
   <si>
-    <t>HO_CAN/motorMeasurements</t>
+    <t>Bus 1 (Controls) (IDs 130-149)</t>
   </si>
   <si>
-    <t>HO_CAN/motorControlSlow</t>
+    <t>Bus 2 (Data) (IDs 100 - 149)</t>
   </si>
   <si>
-    <t>HO_CAN/rawInputs</t>
+    <t>135-140</t>
   </si>
   <si>
-    <t>HO_CAN/motorControlFast</t>
-  </si>
-  <si>
-    <t>HO_CAN/modes</t>
+    <t>Raw ADC readings</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -87,7 +93,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -95,12 +101,394 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,21 +768,235 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E0C7290-1258-4296-A218-99ADFCAFEDCE}">
+  <dimension ref="B1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="47">
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D34"/>
+  <dimension ref="B2:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -402,248 +1004,176 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>11</v>
       </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>12</v>
       </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>13</v>
       </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>14</v>
       </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>15</v>
       </c>
-      <c r="C18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>16</v>
       </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Add ADC CAN outputs
</commit_message>
<xml_diff>
--- a/matlab_code/F28379D/F28379D_benchTest/CANmailboxUsage.xlsx
+++ b/matlab_code/F28379D/F28379D_benchTest/CANmailboxUsage.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ETC-Development\matlab_code\F28379D\F28379D_benchTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99784EA2-2331-47DB-9781-DFA291D4E138}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E71BA1-D1A8-4E07-8B2F-E51762459DD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAN IDs" sheetId="2" r:id="rId1"/>
-    <sheet name="Mailboxes" sheetId="1" r:id="rId2"/>
+    <sheet name="Mailboxes (CANA)" sheetId="1" r:id="rId2"/>
+    <sheet name="Mailboxes (CANB)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>Mailbox Number</t>
   </si>
@@ -63,6 +64,15 @@
   <si>
     <t>Raw ADC readings</t>
   </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>CPU1</t>
+  </si>
+  <si>
+    <t>HO_CAN-&gt;rawInputs</t>
+  </si>
 </sst>
 </file>
 
@@ -414,6 +424,60 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -433,60 +497,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -771,163 +781,202 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E0C7290-1258-4296-A218-99ADFCAFEDCE}">
   <dimension ref="B1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
     </row>
     <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="4" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="21"/>
+      <c r="F4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="20"/>
+      <c r="H4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="16"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="16"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="17" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="16"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="16"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="16"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="16"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="16"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="24"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:G13"/>
@@ -936,45 +985,6 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -985,7 +995,7 @@
   <dimension ref="B2:E34"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,4 +1201,235 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F628C3B-2BBA-463F-AD89-2270FC1F02A4}">
+  <dimension ref="B2:E34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add in system control and basic PWM control
</commit_message>
<xml_diff>
--- a/matlab_code/F28379D/F28379D_benchTest/CANmailboxUsage.xlsx
+++ b/matlab_code/F28379D/F28379D_benchTest/CANmailboxUsage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ETC-Development\matlab_code\F28379D\F28379D_benchTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E71BA1-D1A8-4E07-8B2F-E51762459DD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D103483-BDD5-4694-8097-F6836B8CA6AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAN IDs" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
   <si>
     <t>Mailbox Number</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>HO_CAN-&gt;rawInputs</t>
+  </si>
+  <si>
+    <t>HO_CAN-&gt;modes</t>
+  </si>
+  <si>
+    <t>HO_CAN-&gt;motorControlSlow</t>
   </si>
 </sst>
 </file>
@@ -424,6 +430,45 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -436,6 +481,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -446,57 +503,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -789,162 +795,187 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="21"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="22" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="24"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="25" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="19" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="25" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="21"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="18"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="3"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="4" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
+      <c r="G8" s="15"/>
+      <c r="H8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="16"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="3"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="16"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="16"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="16"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="16"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="3"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="16"/>
     </row>
     <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
@@ -953,38 +984,13 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1208,7 +1214,7 @@
   <dimension ref="B2:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1293,20 +1299,56 @@
       <c r="B7">
         <v>4</v>
       </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add new CAN messages
</commit_message>
<xml_diff>
--- a/matlab_code/F28379D/F28379D_benchTest/CANmailboxUsage.xlsx
+++ b/matlab_code/F28379D/F28379D_benchTest/CANmailboxUsage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ETC-Development\matlab_code\F28379D\F28379D_benchTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D103483-BDD5-4694-8097-F6836B8CA6AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F5B6E5-7BDC-4F3E-BD25-D0C1F8BAA854}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAN IDs" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="28">
   <si>
     <t>Mailbox Number</t>
   </si>
@@ -71,13 +71,46 @@
     <t>CPU1</t>
   </si>
   <si>
-    <t>HO_CAN-&gt;rawInputs</t>
-  </si>
-  <si>
-    <t>HO_CAN-&gt;modes</t>
-  </si>
-  <si>
-    <t>HO_CAN-&gt;motorControlSlow</t>
+    <t>HO_CAN-&gt;CAN2-&gt;modes</t>
+  </si>
+  <si>
+    <t>HO_CAN-&gt;CAN2-&gt;motorControlSlow</t>
+  </si>
+  <si>
+    <t>HO_CAN-&gt;CAN2-&gt;rawInputs</t>
+  </si>
+  <si>
+    <t>130-134</t>
+  </si>
+  <si>
+    <t>Input Readings</t>
+  </si>
+  <si>
+    <t>BP1</t>
+  </si>
+  <si>
+    <t>BP2</t>
+  </si>
+  <si>
+    <t>IO1</t>
+  </si>
+  <si>
+    <t>IO2</t>
+  </si>
+  <si>
+    <t>IO3</t>
+  </si>
+  <si>
+    <t>IO4</t>
+  </si>
+  <si>
+    <t>IO5</t>
+  </si>
+  <si>
+    <t>IO6</t>
+  </si>
+  <si>
+    <t>HO_CAN-&gt;CAN2-&gt;analogInputs</t>
   </si>
 </sst>
 </file>
@@ -430,6 +463,60 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -449,60 +536,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -785,165 +818,272 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E0C7290-1258-4296-A218-99ADFCAFEDCE}">
-  <dimension ref="B1:I14"/>
+  <dimension ref="B1:Q24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:I8"/>
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
+    </row>
+    <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="4" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="24"/>
+    </row>
+    <row r="4" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="21"/>
+      <c r="F4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="20"/>
+      <c r="H4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="16"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="16"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="17" t="s">
+      <c r="I4" s="21"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="18"/>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="16"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="16"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="16"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="16"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="16"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="16"/>
-    </row>
-    <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="24"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>4</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>4</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>4</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <v>4</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <v>5</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P22">
+        <v>5</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P23">
+        <v>5</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="16:17" x14ac:dyDescent="0.25">
+      <c r="P24">
+        <v>5</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:G13"/>
@@ -952,45 +1092,6 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1214,7 +1315,7 @@
   <dimension ref="B2:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,7 +1351,7 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -1264,7 +1365,7 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -1278,7 +1379,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -1292,7 +1393,7 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -1306,7 +1407,7 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -1320,7 +1421,7 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -1334,7 +1435,7 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -1348,37 +1449,91 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9</v>
       </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>11</v>
       </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>12</v>
       </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>13</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix input signals and get temp diodes working
</commit_message>
<xml_diff>
--- a/matlab_code/F28379D/F28379D_benchTest/CANmailboxUsage.xlsx
+++ b/matlab_code/F28379D/F28379D_benchTest/CANmailboxUsage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ETC-Development\matlab_code\F28379D\F28379D_benchTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F5B6E5-7BDC-4F3E-BD25-D0C1F8BAA854}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD74C30-5F6D-4FB5-901E-FD5B7D0635ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAN IDs" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="21">
   <si>
     <t>Mailbox Number</t>
   </si>
@@ -86,31 +86,10 @@
     <t>Input Readings</t>
   </si>
   <si>
-    <t>BP1</t>
-  </si>
-  <si>
-    <t>BP2</t>
-  </si>
-  <si>
-    <t>IO1</t>
-  </si>
-  <si>
-    <t>IO2</t>
-  </si>
-  <si>
-    <t>IO3</t>
-  </si>
-  <si>
-    <t>IO4</t>
-  </si>
-  <si>
-    <t>IO5</t>
-  </si>
-  <si>
-    <t>IO6</t>
-  </si>
-  <si>
     <t>HO_CAN-&gt;CAN2-&gt;analogInputs</t>
+  </si>
+  <si>
+    <t>Board Temp</t>
   </si>
 </sst>
 </file>
@@ -463,6 +442,45 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -475,6 +493,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -485,57 +515,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -818,240 +797,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E0C7290-1258-4296-A218-99ADFCAFEDCE}">
-  <dimension ref="B1:Q24"/>
+  <dimension ref="B1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="21"/>
-    </row>
-    <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="22" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="24"/>
-    </row>
-    <row r="4" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="19" t="s">
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="25" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="19" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="25" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="21"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="18"/>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="4" t="s">
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="G7" s="15"/>
+      <c r="H7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="4" t="s">
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
+      <c r="G8" s="15"/>
+      <c r="H8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="P16">
-        <v>4</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P17">
-        <v>4</v>
-      </c>
-      <c r="Q17" t="s">
+      <c r="I8" s="16"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="17">
+        <v>141</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P19">
-        <v>4</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P20">
-        <v>4</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P21">
-        <v>5</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P22">
-        <v>5</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P23">
-        <v>5</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="16:17" x14ac:dyDescent="0.25">
-      <c r="P24">
-        <v>5</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>26</v>
-      </c>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="16"/>
+    </row>
+    <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
@@ -1060,38 +1004,13 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1315,7 +1234,7 @@
   <dimension ref="B2:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="C17" sqref="C17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,7 +1396,7 @@
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -1491,7 +1410,7 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -1505,7 +1424,7 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -1519,7 +1438,7 @@
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
@@ -1533,85 +1452,94 @@
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Add in motor model
</commit_message>
<xml_diff>
--- a/matlab_code/F28379D/F28379D_benchTest/CANmailboxUsage.xlsx
+++ b/matlab_code/F28379D/F28379D_benchTest/CANmailboxUsage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ETC-Development\matlab_code\F28379D\F28379D_benchTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD74C30-5F6D-4FB5-901E-FD5B7D0635ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CC1E80-9A27-445F-AAF0-B1D9CDD7F918}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAN IDs" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="22">
   <si>
     <t>Mailbox Number</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Board Temp</t>
+  </si>
+  <si>
+    <t>HO_CAN-&gt;CAN2-&gt;motorModel</t>
   </si>
 </sst>
 </file>
@@ -442,6 +445,60 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -461,60 +518,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -807,163 +810,202 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
     </row>
     <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="4" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="24"/>
     </row>
     <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="20"/>
+      <c r="D4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="1" t="s">
+      <c r="E4" s="21"/>
+      <c r="F4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="7" t="s">
+      <c r="G4" s="20"/>
+      <c r="H4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="18"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="14"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="16"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="17" t="s">
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="16"/>
+      <c r="I7" s="3"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="17" t="s">
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="16"/>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="17">
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="4">
         <v>141</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15" t="s">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="16"/>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="16"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="16"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="3"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="16"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="3"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="16"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="3"/>
     </row>
     <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="24"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:G13"/>
@@ -972,45 +1014,6 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1234,7 +1237,7 @@
   <dimension ref="B2:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:E17"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,6 +1476,15 @@
       <c r="B18">
         <v>15</v>
       </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19">

</xml_diff>

<commit_message>
Add position control to model
</commit_message>
<xml_diff>
--- a/matlab_code/F28379D/F28379D_benchTest/CANmailboxUsage.xlsx
+++ b/matlab_code/F28379D/F28379D_benchTest/CANmailboxUsage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\ETC-Development\matlab_code\F28379D\F28379D_benchTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CC1E80-9A27-445F-AAF0-B1D9CDD7F918}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D17E8A6-8863-42BA-B101-421437BCA7F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="23">
   <si>
     <t>Mailbox Number</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>HO_CAN-&gt;CAN2-&gt;motorModel</t>
+  </si>
+  <si>
+    <t>HO_CAN-&gt;CAN2-&gt;motorControlFast</t>
   </si>
 </sst>
 </file>
@@ -445,6 +448,45 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -457,6 +499,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -467,57 +521,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -810,170 +813,195 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="21"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3"/>
     </row>
     <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="22" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="24"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="25" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="19" t="s">
+      <c r="E4" s="3"/>
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="25" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="21"/>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="18"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="3"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="4" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="G7" s="15"/>
+      <c r="H7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="4" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
+      <c r="G8" s="15"/>
+      <c r="H8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="3"/>
+      <c r="I8" s="16"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="4">
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="17">
         <v>141</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
+      <c r="G9" s="15"/>
+      <c r="H9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="3"/>
+      <c r="I9" s="16"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="16"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="16"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="16"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="3"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="16"/>
     </row>
     <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
@@ -982,38 +1010,13 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1237,7 +1240,7 @@
   <dimension ref="B2:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,15 +1493,42 @@
       <c r="B19">
         <v>16</v>
       </c>
+      <c r="C19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>17</v>
       </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>